<commit_message>
project refactored with app name: e-kanban
</commit_message>
<xml_diff>
--- a/data/Product Upload Template.xlsx
+++ b/data/Product Upload Template.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -462,9 +462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -608,5 +608,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>